<commit_message>
the first home commit
</commit_message>
<xml_diff>
--- a/ratsiony.xlsx
+++ b/ratsiony.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="165" yWindow="-135" windowWidth="18540" windowHeight="6690" activeTab="7"/>
@@ -239,11 +239,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,7 +515,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -550,7 +549,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -726,14 +724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="S2" sqref="S2:T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -741,7 +739,7 @@
     <col min="4" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -770,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -783,7 +781,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -815,12 +813,8 @@
         <f t="shared" ref="I3:I18" si="1">(B3*4+C3*4+D3*9)*E3/100</f>
         <v>231.99</v>
       </c>
-      <c r="S3">
-        <f>E3*3</f>
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -852,12 +846,8 @@
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S18" si="3">E4*3</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
@@ -869,12 +859,8 @@
       <c r="G5" s="35"/>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
-      <c r="S5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -895,23 +881,19 @@
         <v>24</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" ref="G6:H6" si="4">C6*$E$6/100</f>
+        <f t="shared" ref="G6:H6" si="3">C6*$E$6/100</f>
         <v>52</v>
       </c>
       <c r="H6" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="1"/>
         <v>317.5</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>23</v>
       </c>
@@ -932,23 +914,19 @@
         <v>18</v>
       </c>
       <c r="G7" s="17">
-        <f t="shared" ref="G7:H7" si="5">C7*$E$7/100</f>
+        <f t="shared" ref="G7:H7" si="4">C7*$E$7/100</f>
         <v>1.5</v>
       </c>
       <c r="H7" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>294</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="35" t="s">
         <v>22</v>
       </c>
@@ -960,12 +938,8 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
-      <c r="S8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -994,15 +968,11 @@
         <v>5.4</v>
       </c>
       <c r="I9" s="16">
-        <f t="shared" ref="I9:I13" si="6">(B9*4+C9*4+D9*9)*E9/100</f>
+        <f t="shared" ref="I9:I13" si="5">(B9*4+C9*4+D9*9)*E9/100</f>
         <v>67.8</v>
       </c>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1031,15 +1001,11 @@
         <v>0.52</v>
       </c>
       <c r="I10" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>79.239999999999981</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1068,15 +1034,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1105,15 +1067,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="I12" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1142,15 +1100,11 @@
         <v>6.3</v>
       </c>
       <c r="I13" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>128.69999999999999</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -1162,12 +1116,8 @@
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-      <c r="S14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1188,23 +1138,19 @@
         <v>1.4</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" ref="G15:H15" si="7">C15*$E$15/100</f>
+        <f t="shared" ref="G15:H15" si="6">C15*$E$15/100</f>
         <v>114.8</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I15" s="16">
         <f t="shared" si="1"/>
         <v>464.8</v>
       </c>
-      <c r="S15">
-        <f t="shared" si="3"/>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="18.75">
       <c r="A16" s="35" t="s">
         <v>19</v>
       </c>
@@ -1216,12 +1162,8 @@
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
-      <c r="S16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1242,23 +1184,19 @@
         <v>13</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" ref="G17:H17" si="8">C17*$E$17/100</f>
+        <f t="shared" ref="G17:H17" si="7">C17*$E$17/100</f>
         <v>89.375</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.375</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>421.875</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1279,23 +1217,19 @@
         <v>12</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" ref="G18:H18" si="9">C18*$E$18/100</f>
+        <f t="shared" ref="G18:H18" si="8">C18*$E$18/100</f>
         <v>1</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="I18" s="16">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="18.75">
       <c r="A19" s="35" t="s">
         <v>20</v>
       </c>
@@ -1308,7 +1242,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -1329,19 +1263,19 @@
         <v>30.5</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" ref="G20:H20" si="10">C20*$E$20/100</f>
+        <f t="shared" ref="G20:H20" si="9">C20*$E$20/100</f>
         <v>111</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" ref="I20" si="11">(B20*4+C20*4+D20*9)*E20/100</f>
+        <f t="shared" ref="I20" si="10">(B20*4+C20*4+D20*9)*E20/100</f>
         <v>781.99999999999989</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
@@ -1366,7 +1300,7 @@
         <v>3430.9049999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -1391,7 +1325,7 @@
         <v>3430.9049999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="10"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1404,16 +1338,16 @@
         <v>15.264777077768112</v>
       </c>
       <c r="G23" s="15">
-        <f t="shared" ref="G23:H23" si="12">G22/($F$22+$G$22+$H$22)*100</f>
+        <f t="shared" ref="G23:H23" si="11">G22/($F$22+$G$22+$H$22)*100</f>
         <v>60.474422929227124</v>
       </c>
       <c r="H23" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>24.260799993004763</v>
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
@@ -1422,15 +1356,15 @@
         <v>2.0457812500000001</v>
       </c>
       <c r="G24" s="21">
-        <f t="shared" ref="G24:H24" si="13">G21/$A$1</f>
+        <f t="shared" ref="G24:H24" si="12">G21/$A$1</f>
         <v>8.1047656249999989</v>
       </c>
       <c r="H24" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.445078125</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1454,14 +1388,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="R3" sqref="R3:T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -1469,7 +1403,7 @@
     <col min="4" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -1498,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -1511,7 +1445,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -1543,12 +1477,8 @@
         <f t="shared" ref="I3:I18" si="1">(B3*4+C3*4+D3*9)*E3/100</f>
         <v>231.99</v>
       </c>
-      <c r="S3">
-        <f>E3*3</f>
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -1580,12 +1510,8 @@
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S20" si="3">E4*3</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
@@ -1597,12 +1523,8 @@
       <c r="G5" s="35"/>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
-      <c r="S5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1623,23 +1545,19 @@
         <v>12.5</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" ref="G6:H6" si="4">C6*$E$6/100</f>
+        <f t="shared" ref="G6:H6" si="3">C6*$E$6/100</f>
         <v>88.75</v>
       </c>
       <c r="H6" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.875</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="1"/>
         <v>421.875</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>23</v>
       </c>
@@ -1660,23 +1578,19 @@
         <v>12</v>
       </c>
       <c r="G7" s="17">
-        <f t="shared" ref="G7:H7" si="5">C7*$E$7/100</f>
+        <f t="shared" ref="G7:H7" si="4">C7*$E$7/100</f>
         <v>0.1</v>
       </c>
       <c r="H7" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>192.4</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="35" t="s">
         <v>22</v>
       </c>
@@ -1688,12 +1602,8 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
-      <c r="S8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1722,15 +1632,11 @@
         <v>5.4</v>
       </c>
       <c r="I9" s="25">
-        <f t="shared" ref="I9:I13" si="6">(B9*4+C9*4+D9*9)*E9/100</f>
+        <f t="shared" ref="I9:I13" si="5">(B9*4+C9*4+D9*9)*E9/100</f>
         <v>67.8</v>
       </c>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1759,15 +1665,11 @@
         <v>0.52</v>
       </c>
       <c r="I10" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>79.239999999999981</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1796,15 +1698,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1833,15 +1731,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="I12" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1870,15 +1764,11 @@
         <v>6.3</v>
       </c>
       <c r="I13" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>128.69999999999999</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -1890,12 +1780,8 @@
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-      <c r="S14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1916,23 +1802,19 @@
         <v>1.35</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" ref="G15:H15" si="7">C15*$E$15/100</f>
+        <f t="shared" ref="G15:H15" si="6">C15*$E$15/100</f>
         <v>109.35</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I15" s="16">
         <f t="shared" si="1"/>
         <v>442.8</v>
       </c>
-      <c r="S15">
-        <f t="shared" si="3"/>
-        <v>405</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="18.75">
       <c r="A16" s="35" t="s">
         <v>19</v>
       </c>
@@ -1944,12 +1826,8 @@
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
-      <c r="S16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1970,23 +1848,19 @@
         <v>7.7</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" ref="G17:H17" si="8">C17*$E$17/100</f>
+        <f t="shared" ref="G17:H17" si="7">C17*$E$17/100</f>
         <v>84.7</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>369.6</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="3"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="3" t="s">
         <v>68</v>
       </c>
@@ -2007,23 +1881,19 @@
         <v>18</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" ref="G18:H18" si="9">C18*$E$18/100</f>
+        <f t="shared" ref="G18:H18" si="8">C18*$E$18/100</f>
         <v>0.15</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="I18" s="16">
         <f t="shared" si="1"/>
         <v>288.60000000000002</v>
       </c>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="18.75">
       <c r="A19" s="35" t="s">
         <v>20</v>
       </c>
@@ -2035,12 +1905,8 @@
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
-      <c r="S19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -2061,23 +1927,19 @@
         <v>30.5</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" ref="G20:H20" si="10">C20*$E$20/100</f>
+        <f t="shared" ref="G20:H20" si="9">C20*$E$20/100</f>
         <v>111</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" ref="I20" si="11">(B20*4+C20*4+D20*9)*E20/100</f>
+        <f t="shared" ref="I20" si="10">(B20*4+C20*4+D20*9)*E20/100</f>
         <v>781.99999999999989</v>
       </c>
-      <c r="S20">
-        <f t="shared" si="3"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
@@ -2102,7 +1964,7 @@
         <v>3452.0050000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -2115,7 +1977,7 @@
         <v>456.32</v>
       </c>
       <c r="G22" s="15">
-        <f t="shared" ref="G22" si="12">G21*4</f>
+        <f t="shared" ref="G22" si="11">G21*4</f>
         <v>2172.3199999999997</v>
       </c>
       <c r="H22" s="15">
@@ -2127,7 +1989,7 @@
         <v>3452.0050000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="10"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2140,16 +2002,16 @@
         <v>13.218984329396974</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" ref="G23:H23" si="13">G22/($F$22+$G$22+$H$22)*100</f>
+        <f t="shared" ref="G23:H23" si="12">G22/($F$22+$G$22+$H$22)*100</f>
         <v>62.929225189418894</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>23.851790481184125</v>
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
@@ -2158,15 +2020,15 @@
         <v>1.7825</v>
       </c>
       <c r="G24" s="21">
-        <f t="shared" ref="G24:H24" si="14">G21/$A$1</f>
+        <f t="shared" ref="G24:H24" si="13">G21/$A$1</f>
         <v>8.4856249999999989</v>
       </c>
       <c r="H24" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.429453125</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2190,14 +2052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="R2" sqref="R2:S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -2205,7 +2067,7 @@
     <col min="4" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -2234,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -2247,7 +2109,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -2279,12 +2141,8 @@
         <f t="shared" ref="I3:I18" si="1">(B3*4+C3*4+D3*9)*E3/100</f>
         <v>231.99</v>
       </c>
-      <c r="S3">
-        <f>E3*3</f>
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -2316,12 +2174,8 @@
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S18" si="3">E4*3</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
@@ -2333,12 +2187,8 @@
       <c r="G5" s="35"/>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
-      <c r="S5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2359,23 +2209,19 @@
         <v>7</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" ref="G6:H6" si="4">C6*$E$6/100</f>
+        <f t="shared" ref="G6:H6" si="3">C6*$E$6/100</f>
         <v>77</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="1"/>
         <v>336</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>23</v>
       </c>
@@ -2396,23 +2242,19 @@
         <v>18</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:H7" si="5">C7*$E$7/100</f>
+        <f t="shared" ref="G7:H7" si="4">C7*$E$7/100</f>
         <v>0.15</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I7" s="19">
         <f t="shared" si="1"/>
         <v>288.60000000000002</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="35" t="s">
         <v>22</v>
       </c>
@@ -2424,12 +2266,8 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
-      <c r="S8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -2458,15 +2296,11 @@
         <v>5.4</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" ref="I9:I13" si="6">(B9*4+C9*4+D9*9)*E9/100</f>
+        <f t="shared" ref="I9:I13" si="5">(B9*4+C9*4+D9*9)*E9/100</f>
         <v>67.8</v>
       </c>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2495,15 +2329,11 @@
         <v>0.52</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>79.239999999999981</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -2532,15 +2362,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -2569,15 +2395,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -2606,15 +2428,11 @@
         <v>6.3</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>128.69999999999999</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -2626,12 +2444,8 @@
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-      <c r="S14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -2652,23 +2466,19 @@
         <v>1.4</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" ref="G15:H15" si="7">C15*$E$15/100</f>
+        <f t="shared" ref="G15:H15" si="6">C15*$E$15/100</f>
         <v>114.8</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="1"/>
         <v>464.8</v>
       </c>
-      <c r="S15">
-        <f t="shared" si="3"/>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="18.75">
       <c r="A16" s="35" t="s">
         <v>19</v>
       </c>
@@ -2680,12 +2490,8 @@
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
-      <c r="S16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -2706,23 +2512,19 @@
         <v>13</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" ref="G17:H17" si="8">C17*$E$17/100</f>
+        <f t="shared" ref="G17:H17" si="7">C17*$E$17/100</f>
         <v>89.375</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.375</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
         <v>421.875</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -2743,23 +2545,19 @@
         <v>29.25</v>
       </c>
       <c r="G18" s="11">
-        <f t="shared" ref="G18:H18" si="9">C18*$E$18/100</f>
+        <f t="shared" ref="G18:H18" si="8">C18*$E$18/100</f>
         <v>0.15</v>
       </c>
       <c r="H18" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="1"/>
         <v>171.6</v>
       </c>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="18.75">
       <c r="A19" s="35" t="s">
         <v>20</v>
       </c>
@@ -2772,7 +2570,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -2793,19 +2591,19 @@
         <v>30.5</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" ref="G20:H20" si="10">C20*$E$20/100</f>
+        <f t="shared" ref="G20:H20" si="9">C20*$E$20/100</f>
         <v>111</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" ref="I20" si="11">(B20*4+C20*4+D20*9)*E20/100</f>
+        <f t="shared" ref="I20" si="10">(B20*4+C20*4+D20*9)*E20/100</f>
         <v>781.99999999999989</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
@@ -2830,7 +2628,7 @@
         <v>3419.605</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -2855,7 +2653,7 @@
         <v>3419.6049999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="10"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2868,16 +2666,16 @@
         <v>15.344462299008221</v>
       </c>
       <c r="G23" s="15">
-        <f t="shared" ref="G23:H23" si="12">G22/($F$22+$G$22+$H$22)*100</f>
+        <f t="shared" ref="G23:H23" si="11">G22/($F$22+$G$22+$H$22)*100</f>
         <v>63.341233855957057</v>
       </c>
       <c r="H23" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>21.314303845034736</v>
       </c>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
@@ -2886,15 +2684,15 @@
         <v>2.0496875000000001</v>
       </c>
       <c r="G24" s="21">
-        <f t="shared" ref="G24:H24" si="13">G21/$A$1</f>
+        <f t="shared" ref="G24:H24" si="12">G21/$A$1</f>
         <v>8.4610156249999999</v>
       </c>
       <c r="H24" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.265390625</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2918,14 +2716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="R2" sqref="R2:T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -2933,7 +2731,7 @@
     <col min="4" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -2962,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -2975,7 +2773,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -3007,12 +2805,8 @@
         <f t="shared" ref="I3:I18" si="1">(B3*4+C3*4+D3*9)*E3/100</f>
         <v>231.99</v>
       </c>
-      <c r="S3">
-        <f>E3*3</f>
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -3044,12 +2838,8 @@
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S20" si="3">E4*3</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
@@ -3061,12 +2851,8 @@
       <c r="G5" s="35"/>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
-      <c r="S5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -3087,23 +2873,19 @@
         <v>12.5</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" ref="G6:H6" si="4">C6*$E$6/100</f>
+        <f t="shared" ref="G6:H6" si="3">C6*$E$6/100</f>
         <v>88.75</v>
       </c>
       <c r="H6" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.875</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="1"/>
         <v>421.875</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -3124,23 +2906,19 @@
         <v>29.25</v>
       </c>
       <c r="G7" s="17">
-        <f t="shared" ref="G7:H7" si="5">C7*$E$7/100</f>
+        <f t="shared" ref="G7:H7" si="4">C7*$E$7/100</f>
         <v>0.15</v>
       </c>
       <c r="H7" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>171.6</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="35" t="s">
         <v>22</v>
       </c>
@@ -3152,12 +2930,8 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
-      <c r="S8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -3186,15 +2960,11 @@
         <v>5.4</v>
       </c>
       <c r="I9" s="25">
-        <f t="shared" ref="I9:I13" si="6">(B9*4+C9*4+D9*9)*E9/100</f>
+        <f t="shared" ref="I9:I13" si="5">(B9*4+C9*4+D9*9)*E9/100</f>
         <v>67.8</v>
       </c>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -3223,15 +2993,11 @@
         <v>0.52</v>
       </c>
       <c r="I10" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>79.239999999999981</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -3260,15 +3026,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -3297,15 +3059,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="I12" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -3334,15 +3092,11 @@
         <v>6.3</v>
       </c>
       <c r="I13" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>128.69999999999999</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -3354,12 +3108,8 @@
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-      <c r="S14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -3380,23 +3130,19 @@
         <v>1.35</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" ref="G15:H15" si="7">C15*$E$15/100</f>
+        <f t="shared" ref="G15:H15" si="6">C15*$E$15/100</f>
         <v>109.35</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I15" s="16">
         <f t="shared" si="1"/>
         <v>442.8</v>
       </c>
-      <c r="S15">
-        <f t="shared" si="3"/>
-        <v>405</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="18.75">
       <c r="A16" s="35" t="s">
         <v>19</v>
       </c>
@@ -3408,12 +3154,8 @@
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
-      <c r="S16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -3434,23 +3176,19 @@
         <v>7.7</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" ref="G17:H17" si="8">C17*$E$17/100</f>
+        <f t="shared" ref="G17:H17" si="7">C17*$E$17/100</f>
         <v>84.7</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>369.6</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="3"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -3471,23 +3209,19 @@
         <v>17.875</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" ref="G18:H18" si="9">C18*$E$18/100</f>
+        <f t="shared" ref="G18:H18" si="8">C18*$E$18/100</f>
         <v>0.125</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>13.75</v>
       </c>
       <c r="I18" s="16">
         <f t="shared" si="1"/>
         <v>195.75</v>
       </c>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="18.75">
       <c r="A19" s="35" t="s">
         <v>20</v>
       </c>
@@ -3499,12 +3233,8 @@
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
-      <c r="S19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -3525,23 +3255,19 @@
         <v>30.5</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" ref="G20:H20" si="10">C20*$E$20/100</f>
+        <f t="shared" ref="G20:H20" si="9">C20*$E$20/100</f>
         <v>111</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" ref="I20" si="11">(B20*4+C20*4+D20*9)*E20/100</f>
+        <f t="shared" ref="I20" si="10">(B20*4+C20*4+D20*9)*E20/100</f>
         <v>781.99999999999989</v>
       </c>
-      <c r="S20">
-        <f t="shared" si="3"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
@@ -3566,7 +3292,7 @@
         <v>3338.355</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -3579,7 +3305,7 @@
         <v>524.81999999999994</v>
       </c>
       <c r="G22" s="15">
-        <f t="shared" ref="G22" si="12">G21*4</f>
+        <f t="shared" ref="G22" si="11">G21*4</f>
         <v>2172.42</v>
       </c>
       <c r="H22" s="15">
@@ -3591,7 +3317,7 @@
         <v>3338.3549999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="10"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -3604,16 +3330,16 @@
         <v>15.720916439384066</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" ref="G23:H23" si="13">G22/($F$22+$G$22+$H$22)*100</f>
+        <f t="shared" ref="G23:H23" si="12">G22/($F$22+$G$22+$H$22)*100</f>
         <v>65.074565167575059</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>19.204518393040885</v>
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
@@ -3622,15 +3348,15 @@
         <v>2.0500781249999998</v>
       </c>
       <c r="G24" s="21">
-        <f t="shared" ref="G24:H24" si="14">G21/$A$1</f>
+        <f t="shared" ref="G24:H24" si="13">G21/$A$1</f>
         <v>8.4860156250000003</v>
       </c>
       <c r="H24" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.113046875</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -3654,14 +3380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -3669,7 +3395,7 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -3698,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -3711,7 +3437,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -3744,7 +3470,7 @@
         <v>231.99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
@@ -3777,7 +3503,7 @@
         <v>133.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
@@ -3790,7 +3516,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>59</v>
       </c>
@@ -3823,7 +3549,7 @@
         <v>379.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="3" t="s">
         <v>60</v>
       </c>
@@ -3856,7 +3582,7 @@
         <v>429.6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="35" t="s">
         <v>22</v>
       </c>
@@ -3869,7 +3595,7 @@
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -3902,7 +3628,7 @@
         <v>67.8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -3935,7 +3661,7 @@
         <v>79.239999999999981</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -3968,7 +3694,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -4001,7 +3727,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -4034,7 +3760,7 @@
         <v>167.4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -4047,7 +3773,7 @@
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -4080,7 +3806,7 @@
         <v>459.2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="18.75">
       <c r="A16" s="35" t="s">
         <v>19</v>
       </c>
@@ -4093,7 +3819,7 @@
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -4126,7 +3852,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -4159,7 +3885,7 @@
         <v>318.8</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="18.75">
       <c r="A19" s="35" t="s">
         <v>20</v>
       </c>
@@ -4172,7 +3898,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -4205,7 +3931,7 @@
         <v>784.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
@@ -4230,7 +3956,7 @@
         <v>3722.28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -4255,7 +3981,7 @@
         <v>3722.28</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="10"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -4277,7 +4003,7 @@
       </c>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
@@ -4294,7 +4020,7 @@
         <v>1.8149999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -4318,14 +4044,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="R2" sqref="R2:T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -4333,7 +4059,7 @@
     <col min="4" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -4362,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -4375,7 +4101,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -4407,12 +4133,8 @@
         <f t="shared" ref="I3:I17" si="1">(B3*4+C3*4+D3*9)*E3/100</f>
         <v>287.12</v>
       </c>
-      <c r="S3">
-        <f>E3*3</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -4444,12 +4166,8 @@
         <f t="shared" si="1"/>
         <v>161.75</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S19" si="3">E4*3</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
@@ -4470,11 +4188,11 @@
         <v>0.06</v>
       </c>
       <c r="G5" s="17">
-        <f t="shared" ref="G5:H5" si="4">C5*$E$5/100</f>
+        <f t="shared" ref="G5:H5" si="3">C5*$E$5/100</f>
         <v>8.4</v>
       </c>
       <c r="H5" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="I5" s="16">
@@ -4482,7 +4200,7 @@
         <v>34.559999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75">
       <c r="A6" s="35" t="s">
         <v>17</v>
       </c>
@@ -4494,12 +4212,8 @@
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
-      <c r="S6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -4520,23 +4234,19 @@
         <v>12.5</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" ref="G7:H7" si="5">C7*$E$7/100</f>
+        <f t="shared" ref="G7:H7" si="4">C7*$E$7/100</f>
         <v>88.75</v>
       </c>
       <c r="H7" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.875</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" si="1"/>
         <v>421.875</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
@@ -4557,23 +4267,19 @@
         <v>21.45</v>
       </c>
       <c r="G8" s="17">
-        <f t="shared" ref="G8:H8" si="6">C8*$E$8/100</f>
+        <f t="shared" ref="G8:H8" si="5">C8*$E$8/100</f>
         <v>0.15</v>
       </c>
       <c r="H8" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>16.5</v>
       </c>
       <c r="I8" s="25">
         <f t="shared" si="1"/>
         <v>234.9</v>
       </c>
-      <c r="S8">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="18.75">
       <c r="A9" s="35" t="s">
         <v>62</v>
       </c>
@@ -4585,12 +4291,8 @@
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -4619,15 +4321,11 @@
         <v>10.23</v>
       </c>
       <c r="I10" s="25">
-        <f t="shared" ref="I10:I12" si="7">(B10*4+C10*4+D10*9)*E10/100</f>
+        <f t="shared" ref="I10:I12" si="6">(B10*4+C10*4+D10*9)*E10/100</f>
         <v>144.15</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -4656,15 +4354,11 @@
         <v>0.1</v>
       </c>
       <c r="I11" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>336.9</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -4693,15 +4387,11 @@
         <v>13.75</v>
       </c>
       <c r="I12" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>195.75</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" ht="18.75">
       <c r="A13" s="35" t="s">
         <v>18</v>
       </c>
@@ -4713,12 +4403,8 @@
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="15.75">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -4739,23 +4425,19 @@
         <v>1.35</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" ref="G14:H14" si="8">C14*$E$14/100</f>
+        <f t="shared" ref="G14:H14" si="7">C14*$E$14/100</f>
         <v>109.35</v>
       </c>
       <c r="H14" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I14" s="16">
         <f t="shared" si="1"/>
         <v>442.8</v>
       </c>
-      <c r="S14">
-        <f t="shared" si="3"/>
-        <v>405</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" ht="18.75">
       <c r="A15" s="35" t="s">
         <v>19</v>
       </c>
@@ -4767,12 +4449,8 @@
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
-      <c r="S15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -4793,23 +4471,19 @@
         <v>7.7</v>
       </c>
       <c r="G16" s="12">
-        <f t="shared" ref="G16:H16" si="9">C16*$E$16/100</f>
+        <f t="shared" ref="G16:H16" si="8">C16*$E$16/100</f>
         <v>84.7</v>
       </c>
       <c r="H16" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" si="1"/>
         <v>369.6</v>
       </c>
-      <c r="S16">
-        <f t="shared" si="3"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
@@ -4830,23 +4504,19 @@
         <v>17.875</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" ref="G17:H17" si="10">C17*$E$17/100</f>
+        <f t="shared" ref="G17:H17" si="9">C17*$E$17/100</f>
         <v>0.125</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>13.75</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>195.75</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" ht="18.75">
       <c r="A18" s="35" t="s">
         <v>20</v>
       </c>
@@ -4858,12 +4528,8 @@
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="3" t="s">
         <v>70</v>
       </c>
@@ -4884,23 +4550,19 @@
         <v>33</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" ref="G19:H19" si="11">C19*$E$19/100</f>
+        <f t="shared" ref="G19:H19" si="10">C19*$E$19/100</f>
         <v>3.3</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>15.4</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" ref="I19" si="12">(B19*4+C19*4+D19*9)*E19/100</f>
+        <f t="shared" ref="I19" si="11">(B19*4+C19*4+D19*9)*E19/100</f>
         <v>283.8</v>
       </c>
-      <c r="S19">
-        <f t="shared" si="3"/>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="34" t="s">
         <v>21</v>
       </c>
@@ -4925,7 +4587,7 @@
         <v>3108.9550000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -4938,7 +4600,7 @@
         <v>530.87999999999988</v>
       </c>
       <c r="G21" s="15">
-        <f t="shared" ref="G21" si="13">G20*4</f>
+        <f t="shared" ref="G21" si="12">G20*4</f>
         <v>1885.8400000000001</v>
       </c>
       <c r="H21" s="15">
@@ -4950,7 +4612,7 @@
         <v>3108.9550000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="10"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -4963,16 +4625,16 @@
         <v>17.075834162926121</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" ref="G22:H22" si="14">G21/($F$21+$G$21+$H$21)*100</f>
+        <f t="shared" ref="G22:H22" si="13">G21/($F$21+$G$21+$H$21)*100</f>
         <v>60.658324099255211</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>22.265841737818654</v>
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="E23" s="6" t="s">
         <v>54</v>
       </c>
@@ -4981,15 +4643,15 @@
         <v>2.0737499999999995</v>
       </c>
       <c r="G23" s="21">
-        <f t="shared" ref="G23:H23" si="15">G20/$A$1</f>
+        <f t="shared" ref="G23:H23" si="14">G20/$A$1</f>
         <v>7.3665625000000006</v>
       </c>
       <c r="H23" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.2017968750000001</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -5013,14 +4675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="S3" sqref="S3:S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -5028,7 +4690,7 @@
     <col min="4" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="20">
         <v>64</v>
       </c>
@@ -5057,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
@@ -5070,7 +4732,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -5102,12 +4764,8 @@
         <f t="shared" ref="I3:I17" si="1">(B3*4+C3*4+D3*9)*E3/100</f>
         <v>287.12</v>
       </c>
-      <c r="S3">
-        <f>E3*3</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -5139,12 +4797,8 @@
         <f t="shared" si="1"/>
         <v>161.75</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S19" si="3">E4*3</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
@@ -5165,11 +4819,11 @@
         <v>0.06</v>
       </c>
       <c r="G5" s="17">
-        <f t="shared" ref="G5:H5" si="4">C5*$E$5/100</f>
+        <f t="shared" ref="G5:H5" si="3">C5*$E$5/100</f>
         <v>8.4</v>
       </c>
       <c r="H5" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="I5" s="16">
@@ -5177,7 +4831,7 @@
         <v>34.559999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75">
       <c r="A6" s="35" t="s">
         <v>17</v>
       </c>
@@ -5189,12 +4843,8 @@
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
-      <c r="S6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -5215,23 +4865,19 @@
         <v>12.5</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" ref="G7:H7" si="5">C7*$E$7/100</f>
+        <f t="shared" ref="G7:H7" si="4">C7*$E$7/100</f>
         <v>88.75</v>
       </c>
       <c r="H7" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.875</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" si="1"/>
         <v>421.875</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="33" t="s">
         <v>52</v>
       </c>
@@ -5252,23 +4898,19 @@
         <v>21.45</v>
       </c>
       <c r="G8" s="17">
-        <f t="shared" ref="G8:H8" si="6">C8*$E$8/100</f>
+        <f t="shared" ref="G8:H8" si="5">C8*$E$8/100</f>
         <v>0.15</v>
       </c>
       <c r="H8" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>16.5</v>
       </c>
       <c r="I8" s="25">
         <f t="shared" si="1"/>
         <v>234.9</v>
       </c>
-      <c r="S8">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="18.75">
       <c r="A9" s="35" t="s">
         <v>62</v>
       </c>
@@ -5280,12 +4922,8 @@
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -5314,15 +4952,11 @@
         <v>10.23</v>
       </c>
       <c r="I10" s="25">
-        <f t="shared" ref="I10:I12" si="7">(B10*4+C10*4+D10*9)*E10/100</f>
+        <f t="shared" ref="I10:I12" si="6">(B10*4+C10*4+D10*9)*E10/100</f>
         <v>144.15</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -5351,15 +4985,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>336</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>63</v>
       </c>
@@ -5388,15 +5018,11 @@
         <v>6</v>
       </c>
       <c r="I12" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>171.6</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" ht="18.75">
       <c r="A13" s="35" t="s">
         <v>18</v>
       </c>
@@ -5408,12 +5034,8 @@
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="15.75">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -5434,23 +5056,19 @@
         <v>1.35</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" ref="G14:H14" si="8">C14*$E$14/100</f>
+        <f t="shared" ref="G14:H14" si="7">C14*$E$14/100</f>
         <v>109.35</v>
       </c>
       <c r="H14" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I14" s="16">
         <f t="shared" si="1"/>
         <v>442.8</v>
       </c>
-      <c r="S14">
-        <f t="shared" si="3"/>
-        <v>405</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" ht="18.75">
       <c r="A15" s="35" t="s">
         <v>19</v>
       </c>
@@ -5462,12 +5080,8 @@
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
-      <c r="S15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -5488,23 +5102,19 @@
         <v>7.7</v>
       </c>
       <c r="G16" s="12">
-        <f t="shared" ref="G16:H16" si="9">C16*$E$16/100</f>
+        <f t="shared" ref="G16:H16" si="8">C16*$E$16/100</f>
         <v>84.7</v>
       </c>
       <c r="H16" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" si="1"/>
         <v>369.6</v>
       </c>
-      <c r="S16">
-        <f t="shared" si="3"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -5525,23 +5135,19 @@
         <v>29.25</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" ref="G17:H17" si="10">C17*$E$17/100</f>
+        <f t="shared" ref="G17:H17" si="9">C17*$E$17/100</f>
         <v>0.15</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>171.6</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" ht="18.75">
       <c r="A18" s="35" t="s">
         <v>20</v>
       </c>
@@ -5553,12 +5159,8 @@
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -5579,23 +5181,19 @@
         <v>30.5</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" ref="G19:H19" si="11">C19*$E$19/100</f>
+        <f t="shared" ref="G19:H19" si="10">C19*$E$19/100</f>
         <v>111</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" ref="I19" si="12">(B19*4+C19*4+D19*9)*E19/100</f>
+        <f t="shared" ref="I19" si="11">(B19*4+C19*4+D19*9)*E19/100</f>
         <v>781.99999999999989</v>
       </c>
-      <c r="S19">
-        <f t="shared" si="3"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="34" t="s">
         <v>21</v>
       </c>
@@ -5620,7 +5218,7 @@
         <v>3557.9549999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -5633,7 +5231,7 @@
         <v>611.87999999999988</v>
       </c>
       <c r="G21" s="15">
-        <f t="shared" ref="G21" si="13">G20*4</f>
+        <f t="shared" ref="G21" si="12">G20*4</f>
         <v>2316.84</v>
       </c>
       <c r="H21" s="15">
@@ -5645,7 +5243,7 @@
         <v>3557.9549999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="10"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -5658,16 +5256,16 @@
         <v>17.197519361543357</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" ref="G22:H22" si="14">G21/($F$21+$G$21+$H$21)*100</f>
+        <f t="shared" ref="G22:H22" si="13">G21/($F$21+$G$21+$H$21)*100</f>
         <v>65.117181077332347</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>17.685299561124296</v>
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="E23" s="6" t="s">
         <v>54</v>
       </c>
@@ -5676,15 +5274,15 @@
         <v>2.3901562499999995</v>
       </c>
       <c r="G23" s="21">
-        <f t="shared" ref="G23:H23" si="15">G20/$A$1</f>
+        <f t="shared" ref="G23:H23" si="14">G20/$A$1</f>
         <v>9.0501562500000006</v>
       </c>
       <c r="H23" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.0924218749999999</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -5708,20 +5306,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="28"/>
       <c r="B1" s="29" t="s">
         <v>34</v>
@@ -5734,7 +5332,7 @@
       </c>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="28" t="s">
         <v>31</v>
       </c>
@@ -5751,7 +5349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="28" t="s">
         <v>30</v>
       </c>
@@ -5768,7 +5366,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="28" t="s">
         <v>32</v>
       </c>
@@ -5785,7 +5383,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -5802,7 +5400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="28" t="s">
         <v>40</v>
       </c>
@@ -5819,7 +5417,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="28" t="s">
         <v>9</v>
       </c>
@@ -5836,7 +5434,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="28" t="s">
         <v>44</v>
       </c>
@@ -5853,7 +5451,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="28" t="s">
         <v>27</v>
       </c>
@@ -5870,7 +5468,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="28" t="s">
         <v>12</v>
       </c>
@@ -5887,7 +5485,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="28" t="s">
         <v>29</v>
       </c>
@@ -5904,7 +5502,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="28" t="s">
         <v>24</v>
       </c>
@@ -5921,7 +5519,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="28" t="s">
         <v>55</v>
       </c>
@@ -5938,7 +5536,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="28" t="s">
         <v>66</v>
       </c>
@@ -5955,7 +5553,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="28" t="s">
         <v>51</v>
       </c>
@@ -5972,7 +5570,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="28" t="s">
         <v>60</v>
       </c>
@@ -5989,7 +5587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="28" t="s">
         <v>61</v>
       </c>
@@ -6006,7 +5604,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="28" t="s">
         <v>58</v>
       </c>
@@ -6023,7 +5621,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="28" t="s">
         <v>45</v>
       </c>
@@ -6040,7 +5638,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="28" t="s">
         <v>46</v>
       </c>
@@ -6057,7 +5655,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75">
       <c r="B21" s="31" t="s">
         <v>67</v>
       </c>
@@ -6066,7 +5664,7 @@
         <v>43.969999999999992</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.75">
       <c r="A22" s="36" t="s">
         <v>47</v>
       </c>
@@ -6074,7 +5672,7 @@
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="28" t="s">
         <v>58</v>
       </c>
@@ -6085,7 +5683,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="28" t="s">
         <v>45</v>
       </c>
@@ -6096,7 +5694,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="28" t="s">
         <v>46</v>
       </c>
@@ -6107,7 +5705,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="28" t="s">
         <v>48</v>
       </c>
@@ -6118,7 +5716,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="28"/>
       <c r="B27" s="28" t="s">
         <v>49</v>
@@ -6128,7 +5726,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75">
       <c r="A28" s="28"/>
       <c r="B28" s="28" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
added fruit and vegetables
</commit_message>
<xml_diff>
--- a/ratsiony.xlsx
+++ b/ratsiony.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="-135" windowWidth="18540" windowHeight="6690" activeTab="6"/>
+    <workbookView xWindow="165" yWindow="-135" windowWidth="18540" windowHeight="6690" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="пн" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="76">
   <si>
     <t>калории</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Сыр лёгкий</t>
   </si>
   <si>
-    <t>Томатная паста</t>
-  </si>
-  <si>
     <t>Обед 13:00</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>Кофе</t>
+  </si>
+  <si>
+    <t>Аджика</t>
   </si>
 </sst>
 </file>
@@ -803,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -923,7 +923,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="4">
         <v>24</v>
@@ -1595,10 +1595,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -2123,7 +2123,7 @@
     </row>
     <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4">
         <v>12</v>
@@ -2379,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -3175,10 +3175,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -3965,10 +3965,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -4755,10 +4755,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -4860,7 +4860,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4">
         <v>0.6</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="9" spans="1:11" ht="18.75">
       <c r="A9" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
@@ -5304,7 +5304,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="4">
         <v>15</v>
@@ -5463,7 +5463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -5504,10 +5504,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75">
@@ -5609,7 +5609,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4">
         <v>0.6</v>
@@ -5650,7 +5650,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="37">
         <v>0</v>
@@ -5691,7 +5691,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -5829,7 +5829,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="37">
         <v>0</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="12" spans="1:11" ht="18.75">
       <c r="A12" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
@@ -5967,7 +5967,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4">
         <v>19.5</v>
@@ -6008,7 +6008,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="37">
         <v>0</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.75">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="4">
         <v>19.5</v>
@@ -6243,7 +6243,7 @@
     </row>
     <row r="23" spans="1:11" ht="15.75">
       <c r="A23" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="37">
         <v>0</v>
@@ -6458,8 +6458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6509,7 +6509,7 @@
         <v>2.75</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>57</v>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="29">
         <v>650</v>
@@ -6738,13 +6738,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="28" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B17" s="29">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="C17" s="29">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>35</v>
@@ -6754,15 +6754,9 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="29">
-        <v>300</v>
-      </c>
-      <c r="C18" s="29">
-        <v>1.3</v>
-      </c>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="29" t="s">
         <v>36</v>
       </c>
@@ -6771,15 +6765,9 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="29">
-        <v>200</v>
-      </c>
-      <c r="C19" s="29">
-        <v>1.3</v>
-      </c>
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="29" t="s">
         <v>36</v>
       </c>
@@ -6788,15 +6776,9 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="29">
-        <v>100</v>
-      </c>
-      <c r="C20" s="29">
-        <v>1</v>
-      </c>
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="29" t="s">
         <v>36</v>
       </c>
@@ -6806,11 +6788,11 @@
     </row>
     <row r="21" spans="1:5" ht="15.75">
       <c r="B21" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="32">
         <f>SUM(C2:C20)</f>
-        <v>43.969999999999992</v>
+        <v>40.22</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75">

</xml_diff>